<commit_message>
changes has been made
asd
</commit_message>
<xml_diff>
--- a/SalesData.xlsx
+++ b/SalesData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO T480\Documents\workspace\Kamran_Haq\Weekly_Data_Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamran\Documents\Process Studio Workspace\AI\WDU_Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="456" yWindow="2628" windowWidth="12276" windowHeight="9360"/>
+    <workbookView xWindow="460" yWindow="2630" windowWidth="12280" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>Andrea</t>
   </si>
   <si>
-    <t>Alexander</t>
+    <t>Alexandera</t>
   </si>
 </sst>
 </file>
@@ -1378,17 +1378,17 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="12.6" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.65" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.9140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.5" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.8984375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.8984375" style="1"/>
+    <col min="5" max="7" width="8.9140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.9140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -1405,7 +1405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.6" customHeight="1">
+    <row r="2" spans="1:6" ht="12.65" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1419,31 +1419,31 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.6" customHeight="1">
+    <row r="3" spans="1:6" ht="12.65" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="12.6" customHeight="1">
+    <row r="4" spans="1:6" ht="12.65" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="12.6" customHeight="1">
+    <row r="5" spans="1:6" ht="12.65" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="12.6" customHeight="1">
+    <row r="6" spans="1:6" ht="12.65" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="12.6" customHeight="1">
+    <row r="7" spans="1:6" ht="12.65" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1451,7 +1451,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="12.6" customHeight="1">
+    <row r="8" spans="1:6" ht="12.65" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>

</xml_diff>